<commit_message>
add extension SD c5dfd36f9ee9067edc19f4673896430d3277aeae
</commit_message>
<xml_diff>
--- a/cp-descriptionsummary/ig/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/cp-descriptionsummary/ig/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-24T16:13:07+00:00</t>
+    <t>2025-07-24T16:28:48+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -4144,7 +4144,7 @@
         <v>80</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="AN15" t="s" s="2">
         <v>80</v>

</xml_diff>